<commit_message>
fix srand, edited excel
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -90,7 +90,7 @@
       <name val="Menlo"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,19 +105,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,14 +122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,12 +408,12 @@
   <dimension ref="A3:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -441,12 +427,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3">
-        <v>6.7</v>
+      <c r="B4" s="1">
+        <v>12</v>
       </c>
       <c r="C4" s="1">
         <v>110</v>
@@ -454,16 +440,17 @@
       <c r="D4" s="4">
         <v>19.8</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3">
-        <v>6</v>
+      <c r="B5" s="1">
+        <v>7.4</v>
       </c>
       <c r="C5" s="1">
         <v>70</v>
@@ -471,16 +458,17 @@
       <c r="D5" s="4">
         <v>19.82</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>1.5</v>
+      <c r="B6" s="2">
+        <v>8.6999999999999993</v>
       </c>
       <c r="C6" s="2">
         <v>61</v>
@@ -488,49 +476,51 @@
       <c r="D6" s="4">
         <v>19.794</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3">
-        <v>8.44</v>
-      </c>
-      <c r="C7" s="5">
-        <v>117.405</v>
+      <c r="B7" s="1">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>114</v>
       </c>
       <c r="D7" s="4">
         <v>19.829699999999999</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F7" s="2"/>
     </row>
     <row r="21" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M21" s="6" t="s">
+      <c r="M21" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M22" s="6" t="s">
+      <c r="M22" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M23" s="6" t="s">
+      <c r="M23" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M24" s="6" t="s">
+      <c r="M24" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M25" s="6" t="s">
+      <c r="M25" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>